<commit_message>
atac-seq correction in data_gsk
</commit_message>
<xml_diff>
--- a/inst/extdata/data_gsk.xlsx
+++ b/inst/extdata/data_gsk.xlsx
@@ -3014,18 +3014,6 @@
     <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/K562_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bam</t>
   </si>
   <si>
-    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bigwig/Meg01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR1TR1_edited.bw</t>
-  </si>
-  <si>
-    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/Meg01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR1TR1_edited.bam</t>
-  </si>
-  <si>
-    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bigwig/Meg01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bw</t>
-  </si>
-  <si>
-    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/Meg01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bam</t>
-  </si>
-  <si>
     <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bigwig/UT7_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR1TR1_edited.bw</t>
   </si>
   <si>
@@ -3036,6 +3024,18 @@
   </si>
   <si>
     <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/UT7_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bam</t>
+  </si>
+  <si>
+    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bigwig/MEG01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR1TR1_edited.bw</t>
+  </si>
+  <si>
+    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/MEG01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR1TR1_edited.bam</t>
+  </si>
+  <si>
+    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bigwig/MEG01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bw</t>
+  </si>
+  <si>
+    <t>/GWD/bioinfo/projects/RD-Epigenetics-NetworkData/otar_020/GSK/atac-seq/project_1/bam/MEG01_ATAC_ATAC-Seq_P1Erythroidcelltypes93_ATAC_P1Erythroidcelltypes93_bwa_samse_BR2TR1_edited.bam</t>
   </si>
 </sst>
 </file>
@@ -3425,7 +3425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5236,10 +5236,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="K50" t="s">
-        <v>999</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -5272,10 +5272,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c r="K51" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -5596,10 +5596,10 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="K60" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -5632,10 +5632,10 @@
         <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="K61" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>